<commit_message>
Combined Verification Test Plan Document
</commit_message>
<xml_diff>
--- a/Test Plan/Movie Theatre Test Cases.xlsx
+++ b/Test Plan/Movie Theatre Test Cases.xlsx
@@ -7,16 +7,11 @@
   </sheets>
   <definedNames/>
   <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7miPT4l/gFk5B/986EipAXIb/G9i6A=="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>Test Case Template</t>
   </si>
@@ -287,6 +282,34 @@
   </si>
   <si>
     <t xml:space="preserve">Users could see movie covers and were able to watch the trailers by being redirected to youtube. </t>
+  </si>
+  <si>
+    <t>Admin_Support_10</t>
+  </si>
+  <si>
+    <t>Customer_Support_Module</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>Verify that Admins can help the user issue a refund or edit their purchased ticket</t>
+  </si>
+  <si>
+    <t>Website is Launched and Admin is logged in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Website
+2. Log in as admin
+3. attempt to edit test ticket
+4. attempt to refund test ticket
+</t>
+  </si>
+  <si>
+    <t>Admin should be able to edit the ticket and submit a refund request to the system.</t>
+  </si>
+  <si>
+    <t>The admin was able to edit and send a refund ticket request to the system. The user recieved the refund within 48 hours.</t>
   </si>
 </sst>
 </file>
@@ -319,7 +342,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -336,12 +359,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor rgb="FF92D050"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -395,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -419,14 +436,11 @@
     <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+    <xf borderId="4" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -916,25 +930,25 @@
       <c r="B9" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="14" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="12" t="s">
@@ -942,82 +956,100 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="9">
-        <v>10.0</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="9"/>
+      <c r="A12" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>